<commit_message>
uppdated the dataset so that there are variable names, currently test1 has named variables and ACS has coded variables
</commit_message>
<xml_diff>
--- a/ACS_summery.xlsx
+++ b/ACS_summery.xlsx
@@ -418,25 +418,25 @@
         <v>7746031</v>
       </c>
       <c r="C2">
-        <v>0.5042892288967086</v>
+        <v>0.504</v>
       </c>
       <c r="D2">
-        <v>0.4957107711032915</v>
+        <v>0.496</v>
       </c>
       <c r="E2">
-        <v>0.9485394520109718</v>
+        <v>0.949</v>
       </c>
       <c r="F2">
-        <v>0.0233186518360177</v>
+        <v>0.023</v>
       </c>
       <c r="G2">
-        <v>0.00130260258447197</v>
+        <v>0.001</v>
       </c>
       <c r="H2">
-        <v>0.006845570331438127</v>
+        <v>0.007</v>
       </c>
       <c r="I2">
-        <v>0.0002370246129921246</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -447,25 +447,25 @@
         <v>11029516</v>
       </c>
       <c r="C3">
-        <v>0.4871008845719069</v>
+        <v>0.487</v>
       </c>
       <c r="D3">
-        <v>0.5128991154280931</v>
+        <v>0.513</v>
       </c>
       <c r="E3">
-        <v>0.782516748695047</v>
+        <v>0.783</v>
       </c>
       <c r="F3">
-        <v>0.1249681309678503</v>
+        <v>0.125</v>
       </c>
       <c r="G3">
-        <v>0.002009426342914775</v>
+        <v>0.002</v>
       </c>
       <c r="H3">
-        <v>0.03895701316358759</v>
+        <v>0.039</v>
       </c>
       <c r="I3">
-        <v>0.0003449834063434878</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -566,43 +566,43 @@
         <v>7746031</v>
       </c>
       <c r="C2">
-        <v>0.04994906423689758</v>
+        <v>0.05</v>
       </c>
       <c r="D2">
-        <v>0.05374326542199483</v>
+        <v>0.054</v>
       </c>
       <c r="E2">
-        <v>0.05746852807586234</v>
+        <v>0.057</v>
       </c>
       <c r="F2">
-        <v>0.06212807565577778</v>
+        <v>0.062</v>
       </c>
       <c r="G2">
-        <v>0.05998271889177825</v>
+        <v>0.06</v>
       </c>
       <c r="H2">
-        <v>0.1099032523882231</v>
+        <v>0.11</v>
       </c>
       <c r="I2">
-        <v>0.1109289389624183</v>
+        <v>0.111</v>
       </c>
       <c r="J2">
-        <v>0.1383711219332843</v>
+        <v>0.138</v>
       </c>
       <c r="K2">
-        <v>0.07833108336385435</v>
+        <v>0.078</v>
       </c>
       <c r="L2">
-        <v>0.07609380855821517</v>
+        <v>0.076</v>
       </c>
       <c r="M2">
-        <v>0.1156540685158632</v>
+        <v>0.116</v>
       </c>
       <c r="N2">
-        <v>0.06160664732686972</v>
+        <v>0.062</v>
       </c>
       <c r="O2">
-        <v>0.02583942666896118</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="3">
@@ -613,43 +613,43 @@
         <v>11029516</v>
       </c>
       <c r="C3">
-        <v>0.05678481267899697</v>
+        <v>0.057</v>
       </c>
       <c r="D3">
-        <v>0.05808360040458711</v>
+        <v>0.058</v>
       </c>
       <c r="E3">
-        <v>0.06090965369649946</v>
+        <v>0.061</v>
       </c>
       <c r="F3">
-        <v>0.06338582762833836</v>
+        <v>0.063</v>
       </c>
       <c r="G3">
-        <v>0.06252323311376493</v>
+        <v>0.063</v>
       </c>
       <c r="H3">
-        <v>0.1347845181964467</v>
+        <v>0.135</v>
       </c>
       <c r="I3">
-        <v>0.11805404697722</v>
+        <v>0.118</v>
       </c>
       <c r="J3">
-        <v>0.1321247459997338</v>
+        <v>0.132</v>
       </c>
       <c r="K3">
-        <v>0.07202129268410328</v>
+        <v>0.072</v>
       </c>
       <c r="L3">
-        <v>0.0677490290598427</v>
+        <v>0.06800000000000001</v>
       </c>
       <c r="M3">
-        <v>0.09730798704131713</v>
+        <v>0.097</v>
       </c>
       <c r="N3">
-        <v>0.05143407924699506</v>
+        <v>0.051</v>
       </c>
       <c r="O3">
-        <v>0.02483717327215446</v>
+        <v>0.025</v>
       </c>
     </row>
   </sheetData>
@@ -735,34 +735,34 @@
         <v>3087091</v>
       </c>
       <c r="C2">
-        <v>0.05244581387461529</v>
+        <v>0.052</v>
       </c>
       <c r="D2">
-        <v>0.04706372439296412</v>
+        <v>0.047</v>
       </c>
       <c r="E2">
-        <v>0.1067697712830623</v>
+        <v>0.107</v>
       </c>
       <c r="F2">
-        <v>0.1050908444227916</v>
+        <v>0.105</v>
       </c>
       <c r="G2">
-        <v>0.1431979167442748</v>
+        <v>0.143</v>
       </c>
       <c r="H2">
-        <v>0.1957286001611226</v>
+        <v>0.196</v>
       </c>
       <c r="I2">
-        <v>0.139100531859929</v>
+        <v>0.139</v>
       </c>
       <c r="J2">
-        <v>0.137349692639446</v>
+        <v>0.137</v>
       </c>
       <c r="K2">
-        <v>0.04248109304196086</v>
+        <v>0.042</v>
       </c>
       <c r="L2">
-        <v>0.03077201157983357</v>
+        <v>0.031</v>
       </c>
     </row>
     <row r="3">
@@ -773,34 +773,34 @@
         <v>4335116</v>
       </c>
       <c r="C3">
-        <v>0.05798852902667426</v>
+        <v>0.058</v>
       </c>
       <c r="D3">
-        <v>0.03910852673838486</v>
+        <v>0.039</v>
       </c>
       <c r="E3">
-        <v>0.08555180530347976</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="F3">
-        <v>0.08676330691035719</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="G3">
-        <v>0.1187908235904183</v>
+        <v>0.119</v>
       </c>
       <c r="H3">
-        <v>0.1744100965233687</v>
+        <v>0.174</v>
       </c>
       <c r="I3">
-        <v>0.1327888342549542</v>
+        <v>0.133</v>
       </c>
       <c r="J3">
-        <v>0.1592951607292631</v>
+        <v>0.159</v>
       </c>
       <c r="K3">
-        <v>0.07063225067103164</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="L3">
-        <v>0.074670666252068</v>
+        <v>0.075</v>
       </c>
     </row>
   </sheetData>
@@ -881,31 +881,31 @@
         <v>5551800</v>
       </c>
       <c r="C2">
-        <v>0.03157282322850247</v>
+        <v>0.032</v>
       </c>
       <c r="D2">
-        <v>0.07205753089088224</v>
+        <v>0.072</v>
       </c>
       <c r="E2">
-        <v>0.4540577830613495</v>
+        <v>0.454</v>
       </c>
       <c r="F2">
-        <v>0.1507435426348212</v>
+        <v>0.151</v>
       </c>
       <c r="G2">
-        <v>0.09156345689686228</v>
+        <v>0.092</v>
       </c>
       <c r="H2">
-        <v>0.1281240318455276</v>
+        <v>0.128</v>
       </c>
       <c r="I2">
-        <v>0.07188083144205483</v>
+        <v>0.072</v>
       </c>
       <c r="J2">
-        <v>0.8963696458806153</v>
+        <v>0.896</v>
       </c>
       <c r="K2">
-        <v>0.2000048632875824</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="3">
@@ -916,31 +916,31 @@
         <v>7702053</v>
       </c>
       <c r="C3">
-        <v>0.0329712091048971</v>
+        <v>0.033</v>
       </c>
       <c r="D3">
-        <v>0.06064110439125776</v>
+        <v>0.061</v>
       </c>
       <c r="E3">
-        <v>0.3256739469333696</v>
+        <v>0.326</v>
       </c>
       <c r="F3">
-        <v>0.1606417146181674</v>
+        <v>0.161</v>
       </c>
       <c r="G3">
-        <v>0.08352630136406489</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="H3">
-        <v>0.2028786350859959</v>
+        <v>0.203</v>
       </c>
       <c r="I3">
-        <v>0.1336670885022474</v>
+        <v>0.134</v>
       </c>
       <c r="J3">
-        <v>0.9063876865038452</v>
+        <v>0.906</v>
       </c>
       <c r="K3">
-        <v>0.3365457235882433</v>
+        <v>0.337</v>
       </c>
     </row>
   </sheetData>
@@ -996,10 +996,10 @@
         <v>3087091</v>
       </c>
       <c r="C2">
-        <v>0.7744627547422477</v>
+        <v>0.774</v>
       </c>
       <c r="D2">
-        <v>0.2255372452577524</v>
+        <v>0.226</v>
       </c>
       <c r="E2">
         <v>2.45</v>
@@ -1016,10 +1016,10 @@
         <v>4335116</v>
       </c>
       <c r="C3">
-        <v>0.6851380678164091</v>
+        <v>0.6850000000000001</v>
       </c>
       <c r="D3">
-        <v>0.3148619321835909</v>
+        <v>0.315</v>
       </c>
       <c r="E3">
         <v>2.54</v>
@@ -1151,58 +1151,58 @@
         <v>3087091</v>
       </c>
       <c r="C2">
-        <v>0.8451302536919061</v>
+        <v>0.845</v>
       </c>
       <c r="D2">
-        <v>0.7732392728299878</v>
+        <v>0.773</v>
       </c>
       <c r="E2">
         <v>3087091</v>
       </c>
       <c r="F2">
-        <v>0.3253830223987566</v>
+        <v>0.325</v>
       </c>
       <c r="G2">
-        <v>0.07186992544113537</v>
+        <v>0.072</v>
       </c>
       <c r="H2">
-        <v>0.2057001235143376</v>
+        <v>0.206</v>
       </c>
       <c r="I2">
-        <v>0.2561148991072826</v>
+        <v>0.256</v>
       </c>
       <c r="J2">
-        <v>0.03553377597226645</v>
+        <v>0.036</v>
       </c>
       <c r="K2">
-        <v>0.0882018055185286</v>
+        <v>0.088</v>
       </c>
       <c r="L2">
-        <v>0.0006070439776475653</v>
+        <v>0.001</v>
       </c>
       <c r="M2">
-        <v>0.01275310640340696</v>
+        <v>0.013</v>
       </c>
       <c r="N2">
-        <v>0.003836297666638269</v>
+        <v>0.004</v>
       </c>
       <c r="O2">
-        <v>0.006910065171386266</v>
+        <v>0.007</v>
       </c>
       <c r="P2">
-        <v>0.01184480794378915</v>
+        <v>0.012</v>
       </c>
       <c r="Q2">
-        <v>0.02031815712591563</v>
+        <v>0.02</v>
       </c>
       <c r="R2">
-        <v>0.987273131890184</v>
+        <v>0.987</v>
       </c>
       <c r="S2">
-        <v>0.009083956384829601</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="T2">
-        <v>0.003642911724986403</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="3">
@@ -1213,58 +1213,58 @@
         <v>4335116</v>
       </c>
       <c r="C3">
-        <v>0.888326633012819</v>
+        <v>0.888</v>
       </c>
       <c r="D3">
-        <v>0.8252300515141925</v>
+        <v>0.825</v>
       </c>
       <c r="E3">
         <v>4335116</v>
       </c>
       <c r="F3">
-        <v>0.534347639140452</v>
+        <v>0.534</v>
       </c>
       <c r="G3">
-        <v>0.04479511044225806</v>
+        <v>0.045</v>
       </c>
       <c r="H3">
-        <v>0.2336209688506605</v>
+        <v>0.234</v>
       </c>
       <c r="I3">
-        <v>0.1502554948933316</v>
+        <v>0.15</v>
       </c>
       <c r="J3">
-        <v>0.007661386684923771</v>
+        <v>0.008</v>
       </c>
       <c r="K3">
-        <v>0.01787057139878149</v>
+        <v>0.018</v>
       </c>
       <c r="L3">
-        <v>0.0004913363333299501</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>0.006700628080079056</v>
+        <v>0.007</v>
       </c>
       <c r="N3">
-        <v>0.004256864176183521</v>
+        <v>0.004</v>
       </c>
       <c r="O3">
-        <v>0.00349240943033589</v>
+        <v>0.003</v>
       </c>
       <c r="P3">
-        <v>0.009255346339059901</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="Q3">
-        <v>0.01603832515669708</v>
+        <v>0.016</v>
       </c>
       <c r="R3">
-        <v>0.9850481509606663</v>
+        <v>0.985</v>
       </c>
       <c r="S3">
-        <v>0.01042855600634447</v>
+        <v>0.01</v>
       </c>
       <c r="T3">
-        <v>0.004523293032989198</v>
+        <v>0.005</v>
       </c>
     </row>
   </sheetData>
@@ -1469,91 +1469,91 @@
         <v>1141409</v>
       </c>
       <c r="F2">
-        <v>0.02508047361935049</v>
+        <v>0.025</v>
       </c>
       <c r="G2">
-        <v>0.3119404600199953</v>
+        <v>0.312</v>
       </c>
       <c r="H2">
-        <v>0.356561527391718</v>
+        <v>0.357</v>
       </c>
       <c r="I2">
-        <v>0.1747048762248707</v>
+        <v>0.175</v>
       </c>
       <c r="J2">
-        <v>0.07367474929217133</v>
+        <v>0.074</v>
       </c>
       <c r="K2">
-        <v>0.0305137552148359</v>
+        <v>0.031</v>
       </c>
       <c r="L2">
-        <v>0.0275241582370584</v>
+        <v>0.028</v>
       </c>
       <c r="M2">
         <v>1140</v>
       </c>
       <c r="N2">
-        <v>0.0972987558815593</v>
+        <v>0.097</v>
       </c>
       <c r="O2">
-        <v>0.2999011750537724</v>
+        <v>0.3</v>
       </c>
       <c r="P2">
-        <v>0.3725474884668077</v>
+        <v>0.373</v>
       </c>
       <c r="Q2">
-        <v>0.1501115359687231</v>
+        <v>0.15</v>
       </c>
       <c r="R2">
-        <v>0.0492805908326197</v>
+        <v>0.049</v>
       </c>
       <c r="S2">
-        <v>0.03086045379651779</v>
+        <v>0.031</v>
       </c>
       <c r="T2">
         <v>440</v>
       </c>
       <c r="U2">
-        <v>0.518450730369274</v>
+        <v>0.518</v>
       </c>
       <c r="V2">
-        <v>0.1502961438480138</v>
+        <v>0.15</v>
       </c>
       <c r="W2">
-        <v>0.09445882315750054</v>
+        <v>0.094</v>
       </c>
       <c r="X2">
-        <v>0.06085478454491441</v>
+        <v>0.061</v>
       </c>
       <c r="Y2">
-        <v>0.1759395180802973</v>
+        <v>0.176</v>
       </c>
       <c r="Z2">
-        <v>0.003731080148918976</v>
+        <v>0.004</v>
       </c>
       <c r="AA2">
-        <v>0.426504434431479</v>
+        <v>0.427</v>
       </c>
       <c r="AB2">
-        <v>0.2070046757998229</v>
+        <v>0.207</v>
       </c>
       <c r="AC2">
-        <v>0.1209548899649468</v>
+        <v>0.121</v>
       </c>
       <c r="AD2">
-        <v>0.07424332557391786</v>
+        <v>0.074</v>
       </c>
       <c r="AE2">
-        <v>0.0483954480821511</v>
+        <v>0.048</v>
       </c>
       <c r="AF2">
-        <v>0.03059464223604335</v>
+        <v>0.031</v>
       </c>
       <c r="AG2">
-        <v>0.09230258391163904</v>
+        <v>0.092</v>
       </c>
       <c r="AH2">
-        <v>0.009754610310589806</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="3">
@@ -1573,91 +1573,91 @@
         <v>1107044</v>
       </c>
       <c r="F3">
-        <v>0.008925719529733752</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="G3">
-        <v>0.1566494853997063</v>
+        <v>0.157</v>
       </c>
       <c r="H3">
-        <v>0.2911287049302508</v>
+        <v>0.291</v>
       </c>
       <c r="I3">
-        <v>0.2340424726972427</v>
+        <v>0.234</v>
       </c>
       <c r="J3">
-        <v>0.1397714172680651</v>
+        <v>0.14</v>
       </c>
       <c r="K3">
-        <v>0.07698926265395718</v>
+        <v>0.077</v>
       </c>
       <c r="L3">
-        <v>0.09249293752104422</v>
+        <v>0.092</v>
       </c>
       <c r="M3">
         <v>1471</v>
       </c>
       <c r="N3">
-        <v>0.05125272126884797</v>
+        <v>0.051</v>
       </c>
       <c r="O3">
-        <v>0.1640699645141185</v>
+        <v>0.164</v>
       </c>
       <c r="P3">
-        <v>0.3164931662443007</v>
+        <v>0.316</v>
       </c>
       <c r="Q3">
-        <v>0.2312127527721671</v>
+        <v>0.231</v>
       </c>
       <c r="R3">
-        <v>0.1178409868182541</v>
+        <v>0.118</v>
       </c>
       <c r="S3">
-        <v>0.1191304083823117</v>
+        <v>0.119</v>
       </c>
       <c r="T3">
         <v>567</v>
       </c>
       <c r="U3">
-        <v>0.4806832623727077</v>
+        <v>0.481</v>
       </c>
       <c r="V3">
-        <v>0.1607385693339397</v>
+        <v>0.161</v>
       </c>
       <c r="W3">
-        <v>0.1056996775569431</v>
+        <v>0.106</v>
       </c>
       <c r="X3">
-        <v>0.06505296813663511</v>
+        <v>0.065</v>
       </c>
       <c r="Y3">
-        <v>0.1878255225997745</v>
+        <v>0.188</v>
       </c>
       <c r="Z3">
-        <v>0.004050887613780289</v>
+        <v>0.004</v>
       </c>
       <c r="AA3">
-        <v>0.3966012191024024</v>
+        <v>0.397</v>
       </c>
       <c r="AB3">
-        <v>0.1981890512030236</v>
+        <v>0.198</v>
       </c>
       <c r="AC3">
-        <v>0.1202309935287125</v>
+        <v>0.12</v>
       </c>
       <c r="AD3">
-        <v>0.0777512004942893</v>
+        <v>0.078</v>
       </c>
       <c r="AE3">
-        <v>0.0515688626648986</v>
+        <v>0.052</v>
       </c>
       <c r="AF3">
-        <v>0.03596424351696952</v>
+        <v>0.036</v>
       </c>
       <c r="AG3">
-        <v>0.1196944294897041</v>
+        <v>0.12</v>
       </c>
       <c r="AH3">
-        <v>0.01159664837169977</v>
+        <v>0.012</v>
       </c>
     </row>
   </sheetData>

</xml_diff>